<commit_message>
stat collector to fix lobs and rlsps
</commit_message>
<xml_diff>
--- a/bluejays_2016.xlsx
+++ b/bluejays_2016.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="72" windowWidth="21060" windowHeight="10080" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="72" windowWidth="21060" windowHeight="10080" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="donaj_2016" sheetId="1" r:id="rId1"/>
     <sheet name="donaj Run_Scored" sheetId="2" r:id="rId2"/>
     <sheet name="carre_2016" sheetId="3" r:id="rId3"/>
     <sheet name="carre Run_Scored" sheetId="4" r:id="rId4"/>
+    <sheet name="Team" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">carre_2016!$A$1:$AL$111</definedName>
@@ -20,8 +21,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sinto</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sinto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sinto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+66</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sinto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sinto:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+25</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="328">
   <si>
     <t>Rk</t>
   </si>
@@ -952,12 +1059,66 @@
   <si>
     <t>TOR201609280</t>
   </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>IW</t>
+  </si>
+  <si>
+    <t>LOB</t>
+  </si>
+  <si>
+    <t>RLSP</t>
+  </si>
+  <si>
+    <t>bautj002</t>
+  </si>
+  <si>
+    <t>carre001</t>
+  </si>
+  <si>
+    <t>donaj001</t>
+  </si>
+  <si>
+    <t>encae001</t>
+  </si>
+  <si>
+    <t>goinr001</t>
+  </si>
+  <si>
+    <t>pillk001</t>
+  </si>
+  <si>
+    <t>saunm001</t>
+  </si>
+  <si>
+    <t>smoaj001</t>
+  </si>
+  <si>
+    <t>travd001</t>
+  </si>
+  <si>
+    <t>tulot001</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1092,6 +1253,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1435,11 +1609,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -32858,7 +33033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
@@ -33975,4 +34150,669 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="3">
+        <v>240</v>
+      </c>
+      <c r="C2" s="3">
+        <v>192</v>
+      </c>
+      <c r="D2" s="3">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3">
+        <v>41</v>
+      </c>
+      <c r="F2" s="3">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4">
+        <v>41</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>42</v>
+      </c>
+      <c r="M2" s="3">
+        <v>46</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>150</v>
+      </c>
+      <c r="S2" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" s="3">
+        <v>186</v>
+      </c>
+      <c r="C3" s="3">
+        <v>160</v>
+      </c>
+      <c r="D3" s="3">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>18</v>
+      </c>
+      <c r="M3" s="3">
+        <v>42</v>
+      </c>
+      <c r="N3" s="3">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>5</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>111</v>
+      </c>
+      <c r="S3" s="3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="3">
+        <v>351</v>
+      </c>
+      <c r="C4" s="3">
+        <v>290</v>
+      </c>
+      <c r="D4" s="3">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3">
+        <v>86</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3">
+        <v>58</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>53</v>
+      </c>
+      <c r="M4" s="3">
+        <v>58</v>
+      </c>
+      <c r="N4" s="3">
+        <v>6</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>5</v>
+      </c>
+      <c r="R4" s="3">
+        <v>201</v>
+      </c>
+      <c r="S4" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B5" s="3">
+        <v>338</v>
+      </c>
+      <c r="C5" s="3">
+        <v>284</v>
+      </c>
+      <c r="D5" s="3">
+        <v>48</v>
+      </c>
+      <c r="E5" s="3">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4">
+        <v>67</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>43</v>
+      </c>
+      <c r="M5" s="3">
+        <v>61</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>202</v>
+      </c>
+      <c r="S5" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="3">
+        <v>82</v>
+      </c>
+      <c r="C6" s="3">
+        <v>76</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>63</v>
+      </c>
+      <c r="S6" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" s="3">
+        <v>287</v>
+      </c>
+      <c r="C7" s="3">
+        <v>269</v>
+      </c>
+      <c r="D7" s="3">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3">
+        <v>81</v>
+      </c>
+      <c r="F7" s="3">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>29</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>9</v>
+      </c>
+      <c r="M7" s="3">
+        <v>39</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5</v>
+      </c>
+      <c r="O7" s="3">
+        <v>2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>185</v>
+      </c>
+      <c r="S7" s="3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" s="3">
+        <v>276</v>
+      </c>
+      <c r="C8" s="3">
+        <v>241</v>
+      </c>
+      <c r="D8" s="3">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3">
+        <v>64</v>
+      </c>
+      <c r="F8" s="3">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>32</v>
+      </c>
+      <c r="M8" s="3">
+        <v>82</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="3">
+        <v>177</v>
+      </c>
+      <c r="S8" s="3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" s="3">
+        <v>187</v>
+      </c>
+      <c r="C9" s="3">
+        <v>164</v>
+      </c>
+      <c r="D9" s="3">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3">
+        <v>37</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3">
+        <v>21</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>21</v>
+      </c>
+      <c r="M9" s="3">
+        <v>62</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3">
+        <v>126</v>
+      </c>
+      <c r="S9" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" s="3">
+        <v>200</v>
+      </c>
+      <c r="C10" s="3">
+        <v>187</v>
+      </c>
+      <c r="D10" s="3">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>15</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>11</v>
+      </c>
+      <c r="M10" s="3">
+        <v>40</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>133</v>
+      </c>
+      <c r="S10" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" s="3">
+        <v>270</v>
+      </c>
+      <c r="C11" s="3">
+        <v>242</v>
+      </c>
+      <c r="D11" s="3">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3">
+        <v>63</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>13</v>
+      </c>
+      <c r="I11" s="3">
+        <v>41</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>24</v>
+      </c>
+      <c r="M11" s="3">
+        <v>51</v>
+      </c>
+      <c r="N11" s="3">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3">
+        <v>177</v>
+      </c>
+      <c r="S11" s="3">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>